<commit_message>
add project data partial parse
</commit_message>
<xml_diff>
--- a/pcor_tools/tests/test_resources/pcor_geospatial_data_resource_test1.xlsx
+++ b/pcor_tools/tests/test_resources/pcor_geospatial_data_resource_test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conwaymc/Documents/workspace-pcor/pcor_gen3_artifacts/pcor_tools/tests/test_resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EECED43-A996-3949-BAFB-A6C6DA8F8966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CBD758-DA04-9642-B287-1AF444E247E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="2600" windowWidth="21240" windowHeight="26000" xr2:uid="{0E637B2F-D201-6448-B8F7-9EEB771C5771}"/>
   </bookViews>
@@ -573,7 +573,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <r>
       <rPr>
@@ -753,6 +753,15 @@
   </si>
   <si>
     <t>this is the name</t>
+  </si>
+  <si>
+    <t>proj_sub_id</t>
+  </si>
+  <si>
+    <t>affil</t>
+  </si>
+  <si>
+    <t>inv name</t>
   </si>
 </sst>
 </file>
@@ -1296,7 +1305,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1473,17 +1482,25 @@
       <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="18" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>11</v>
       </c>
+      <c r="B18" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="19" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="B19" s="13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
@@ -1494,39 +1511,59 @@
       <c r="A21" s="12" t="s">
         <v>14</v>
       </c>
+      <c r="B21" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="D21" s="15"/>
     </row>
     <row r="22" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>15</v>
       </c>
+      <c r="B22" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
         <v>16</v>
       </c>
+      <c r="B23" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="D23" s="15"/>
     </row>
     <row r="24" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="B24" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="25" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="14"/>
+      <c r="B25" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>21</v>
       </c>
+      <c r="B26" s="13" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -1703,19 +1740,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f8ccea31-b6eb-442e-9861-83bfaa3f0700" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="820a8b12-53ce-4f8d-a44f-cb0888f07af4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005935BF067F8ACD46B3C6EF2258C28D09" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4e886d676166cb7ae49bec2ac0bf243f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="820a8b12-53ce-4f8d-a44f-cb0888f07af4" xmlns:ns3="f8ccea31-b6eb-442e-9861-83bfaa3f0700" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e226ee36dee42837657b772ac6fcd020" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1975,6 +1999,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f8ccea31-b6eb-442e-9861-83bfaa3f0700" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="820a8b12-53ce-4f8d-a44f-cb0888f07af4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1985,24 +2022,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA4D8767-8400-47FB-8DD5-A41B5BD08C2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f8ccea31-b6eb-442e-9861-83bfaa3f0700"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="820a8b12-53ce-4f8d-a44f-cb0888f07af4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA839343-07D0-489C-B0E9-F9338D36941F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2022,6 +2041,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA4D8767-8400-47FB-8DD5-A41B5BD08C2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f8ccea31-b6eb-442e-9861-83bfaa3f0700"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="820a8b12-53ce-4f8d-a44f-cb0888f07af4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8A970B-FF16-4AB4-B023-04E198ABAD7B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
now parses geo resc
</commit_message>
<xml_diff>
--- a/pcor_tools/tests/test_resources/pcor_geospatial_data_resource_test1.xlsx
+++ b/pcor_tools/tests/test_resources/pcor_geospatial_data_resource_test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conwaymc/Documents/workspace-pcor/pcor_gen3_artifacts/pcor_tools/tests/test_resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B687E2-09FA-E644-948F-E3ABA0182F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE90F61-CC4B-744C-9AE8-A74D1BBEA3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="22400" xr2:uid="{0E637B2F-D201-6448-B8F7-9EEB771C5771}"/>
   </bookViews>
@@ -143,28 +143,15 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">Unique identifier for the project. </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+          </rPr>
+          <t>Unique identifier for the project. Unique name, all caps, dash (-) separated. Example: EPA</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Unique name, all caps, dash (-) separated. Example: EPA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -180,7 +167,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">The date or date range in which the project data was collected.
 </t>
@@ -194,7 +180,6 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Dates are ISO 8601 in the following format (UTC)
 </t>
         </r>
         <r>
@@ -205,6 +190,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">Dates are ISO 8601 in the following format (UTC)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">
 </t>
         </r>
@@ -215,7 +211,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>2023-04-27T18:44:24Z</t>
         </r>
@@ -230,7 +225,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The investigator's affiliation with respect to a research institution.</t>
         </r>
@@ -401,7 +395,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>The ID of the source providing support/grant resources.</t>
         </r>
@@ -493,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{9349C009-77E7-C848-B977-9DAA9FA4DEA0}">
+    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{27A245CB-7193-FE4C-8B44-012C9F44547A}">
       <text>
         <r>
           <rPr>
@@ -503,33 +496,12 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The type of environmental phenomena being observed (e.g., air_pollution, wildfire plumes. Note this is the high level observable, the specific measures contribute to this observation).
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This field supports multiple entries. Place eace entry in successive columns in this row.</t>
+          <t xml:space="preserve">Frequency of time points.
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{A120A261-B3F1-1844-8CF0-EDC84FB618F3}">
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{3A7BD4A1-3B93-F844-A2CC-393B98EC3ED8}">
       <text>
         <r>
           <rPr>
@@ -544,7 +516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A40" authorId="0" shapeId="0" xr:uid="{1F6A870A-05CC-3548-A776-C3C36CA35525}">
+    <comment ref="A44" authorId="0" shapeId="0" xr:uid="{2F9F6380-1FA7-C84A-90F9-7EEE0DAB8413}">
       <text>
         <r>
           <rPr>
@@ -554,33 +526,12 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The type of environmental phenomena being observed (e.g., air_pollution, wildfire plumes. Note this is the high level observable, the specific measures contribute to this observation).
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This field supports multiple entries. Place eace entry in successive columns in this row.</t>
+          <t xml:space="preserve">Frequency of time points.
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{2F9F6380-1FA7-C84A-90F9-7EEE0DAB8413}">
+    <comment ref="A45" authorId="0" shapeId="0" xr:uid="{5C1D102C-FCB3-DE4E-B995-D6B83D8579DD}">
       <text>
         <r>
           <rPr>
@@ -600,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <r>
       <rPr>
@@ -808,12 +759,21 @@
   <si>
     <t># This section describes resource details unique to the specific resource type for this template</t>
   </si>
+  <si>
+    <t>source name</t>
+  </si>
+  <si>
+    <t>source url</t>
+  </si>
+  <si>
+    <t>sub id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -888,21 +848,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -919,6 +864,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1347,16 +1298,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BBD591F-71B4-8D4C-8899-A270C150C296}">
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1655,98 +1606,105 @@
       <c r="A34" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="14"/>
+      <c r="B34" s="14" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+    </row>
+    <row r="44" spans="1:16" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-    </row>
-    <row r="39" spans="1:16" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="12" t="s">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+    </row>
+    <row r="45" spans="1:16" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B45" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C45" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D45" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E45" s="9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B4EE5AA8-C929-464A-A027-12F17FB3CA6E}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$3</xm:f>
@@ -1758,12 +1716,6 @@
             <xm:f>Validation!$B$2:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>B27</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A9B82486-E9B5-1747-B713-76882DCDEE66}">
-          <x14:formula1>
-            <xm:f>Validation!$C$2:$C$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>B36 B41</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
integrate parse result for processing
</commit_message>
<xml_diff>
--- a/pcor_tools/tests/test_resources/pcor_geospatial_data_resource_test1.xlsx
+++ b/pcor_tools/tests/test_resources/pcor_geospatial_data_resource_test1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conwaymc/Documents/workspace-pcor/pcor_gen3_artifacts/pcor_tools/tests/test_resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pateldes/Documents/github/pcor/pcor_gen3_artifacts/pcor_tools/tests/test_resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE90F61-CC4B-744C-9AE8-A74D1BBEA3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3C1D93-4B83-0A48-BC15-FDF945CB0ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="22400" xr2:uid="{0E637B2F-D201-6448-B8F7-9EEB771C5771}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="12120" windowHeight="22400" xr2:uid="{0E637B2F-D201-6448-B8F7-9EEB771C5771}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <r>
       <rPr>
@@ -727,12 +727,6 @@
     <t>temporal resolution</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>this is the name</t>
-  </si>
-  <si>
     <t>proj_sub_id</t>
   </si>
   <si>
@@ -767,6 +761,9 @@
   </si>
   <si>
     <t>sub id</t>
+  </si>
+  <si>
+    <t>NFS</t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BBD591F-71B4-8D4C-8899-A270C150C296}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,7 +1391,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -1402,7 +1399,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -1479,7 +1476,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -1508,7 +1505,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D21" s="15"/>
     </row>
@@ -1517,7 +1514,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" s="15"/>
     </row>
@@ -1607,33 +1604,33 @@
         <v>10</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:16" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1676,16 +1673,16 @@
         <v>31</v>
       </c>
       <c r="B45" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="E45" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -1811,6 +1808,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f8ccea31-b6eb-442e-9861-83bfaa3f0700" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="820a8b12-53ce-4f8d-a44f-cb0888f07af4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005935BF067F8ACD46B3C6EF2258C28D09" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4e886d676166cb7ae49bec2ac0bf243f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="820a8b12-53ce-4f8d-a44f-cb0888f07af4" xmlns:ns3="f8ccea31-b6eb-442e-9861-83bfaa3f0700" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e226ee36dee42837657b772ac6fcd020" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2070,19 +2080,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f8ccea31-b6eb-442e-9861-83bfaa3f0700" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="820a8b12-53ce-4f8d-a44f-cb0888f07af4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2093,6 +2090,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA4D8767-8400-47FB-8DD5-A41B5BD08C2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f8ccea31-b6eb-442e-9861-83bfaa3f0700"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="820a8b12-53ce-4f8d-a44f-cb0888f07af4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA839343-07D0-489C-B0E9-F9338D36941F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2112,24 +2127,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA4D8767-8400-47FB-8DD5-A41B5BD08C2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f8ccea31-b6eb-442e-9861-83bfaa3f0700"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="820a8b12-53ce-4f8d-a44f-cb0888f07af4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8A970B-FF16-4AB4-B023-04E198ABAD7B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update ss for testing
</commit_message>
<xml_diff>
--- a/pcor_tools/tests/test_resources/pcor_geospatial_data_resource_test1.xlsx
+++ b/pcor_tools/tests/test_resources/pcor_geospatial_data_resource_test1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pateldes/Documents/github/pcor/pcor_gen3_artifacts/pcor_tools/tests/test_resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conwaymc/Documents/workspace-pcor/pcor_gen3_artifacts/pcor_tools/tests/test_resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3C1D93-4B83-0A48-BC15-FDF945CB0ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C846E9-60E5-8E46-8ECB-273539500CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="12120" windowHeight="22400" xr2:uid="{0E637B2F-D201-6448-B8F7-9EEB771C5771}"/>
+    <workbookView xWindow="200" yWindow="2580" windowWidth="21240" windowHeight="26000" xr2:uid="{0E637B2F-D201-6448-B8F7-9EEB771C5771}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <r>
       <rPr>
@@ -727,6 +727,12 @@
     <t>temporal resolution</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>this is the name</t>
+  </si>
+  <si>
     <t>proj_sub_id</t>
   </si>
   <si>
@@ -761,9 +767,6 @@
   </si>
   <si>
     <t>sub id</t>
-  </si>
-  <si>
-    <t>NFS</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1301,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1391,7 +1394,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -1399,7 +1402,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -1476,7 +1479,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="13" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -1505,7 +1508,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D21" s="15"/>
     </row>
@@ -1514,7 +1517,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" s="15"/>
     </row>
@@ -1604,33 +1607,33 @@
         <v>10</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:16" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1673,16 +1676,16 @@
         <v>31</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -1808,19 +1811,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f8ccea31-b6eb-442e-9861-83bfaa3f0700" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="820a8b12-53ce-4f8d-a44f-cb0888f07af4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005935BF067F8ACD46B3C6EF2258C28D09" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4e886d676166cb7ae49bec2ac0bf243f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="820a8b12-53ce-4f8d-a44f-cb0888f07af4" xmlns:ns3="f8ccea31-b6eb-442e-9861-83bfaa3f0700" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e226ee36dee42837657b772ac6fcd020" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2080,6 +2070,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f8ccea31-b6eb-442e-9861-83bfaa3f0700" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="820a8b12-53ce-4f8d-a44f-cb0888f07af4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2090,24 +2093,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA4D8767-8400-47FB-8DD5-A41B5BD08C2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f8ccea31-b6eb-442e-9861-83bfaa3f0700"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="820a8b12-53ce-4f8d-a44f-cb0888f07af4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA839343-07D0-489C-B0E9-F9338D36941F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2127,6 +2112,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA4D8767-8400-47FB-8DD5-A41B5BD08C2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f8ccea31-b6eb-442e-9861-83bfaa3f0700"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="820a8b12-53ce-4f8d-a44f-cb0888f07af4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8A970B-FF16-4AB4-B023-04E198ABAD7B}">
   <ds:schemaRefs>

</xml_diff>